<commit_message>
Too many changes to even begin to list. I need to get better about listing all the changes as I go along.
</commit_message>
<xml_diff>
--- a/V1000_Drive_Programmer/data/DRIVE_LIST.xlsx
+++ b/V1000_Drive_Programmer/data/DRIVE_LIST.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2835" yWindow="0" windowWidth="23025" windowHeight="7740"/>
+    <workbookView xWindow="3780" yWindow="0" windowWidth="23025" windowHeight="7740"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="27">
   <si>
     <t>Yaskawa</t>
   </si>
@@ -78,6 +78,33 @@
   </si>
   <si>
     <t>V1000_GRP_DESC</t>
+  </si>
+  <si>
+    <t>UL_DESC</t>
+  </si>
+  <si>
+    <t>VARIABLE FREQUENCY DRIVE, 230V, 5 A</t>
+  </si>
+  <si>
+    <t>VARIABLE FREQUENCY DRIVE, 460V, 3.4 A</t>
+  </si>
+  <si>
+    <t>VARIABLE FREQUENCY DRIVE, 230V, 8 A</t>
+  </si>
+  <si>
+    <t>VARIABLE FREQUENCY DRIVE, 460V, 4.8 A</t>
+  </si>
+  <si>
+    <t>VARIABLE FREQUENCY DRIVE, 230V, 17.5 A</t>
+  </si>
+  <si>
+    <t>VARIABLE FREQUENCY DRIVE, 460V, 9.2 A</t>
+  </si>
+  <si>
+    <t>VARIABLE FREQUENCY DRIVE, 230V, 25 A</t>
+  </si>
+  <si>
+    <t>VARIABLE FREQUENCY DRIVE, 460V, 14.8 A</t>
   </si>
 </sst>
 </file>
@@ -394,23 +421,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -418,19 +446,22 @@
         <v>10</v>
       </c>
       <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -438,19 +469,22 @@
         <v>21520</v>
       </c>
       <c r="C2" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>15</v>
       </c>
-      <c r="F2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -458,19 +492,22 @@
         <v>21521</v>
       </c>
       <c r="C3" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -478,19 +515,22 @@
         <v>21522</v>
       </c>
       <c r="C4" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>15</v>
       </c>
-      <c r="F4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -498,19 +538,22 @@
         <v>21523</v>
       </c>
       <c r="C5" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
         <v>4</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>16</v>
       </c>
-      <c r="F5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -518,19 +561,22 @@
         <v>21524</v>
       </c>
       <c r="C6" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
         <v>5</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>15</v>
       </c>
-      <c r="F6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -538,19 +584,22 @@
         <v>21525</v>
       </c>
       <c r="C7" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
         <v>6</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>16</v>
       </c>
-      <c r="F7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -558,19 +607,22 @@
         <v>21540</v>
       </c>
       <c r="C8" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
         <v>7</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>15</v>
       </c>
-      <c r="F8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -578,15 +630,18 @@
         <v>21541</v>
       </c>
       <c r="C9" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
         <v>8</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>16</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- Commit before starting to figure out how to implement a way to implement a way to compare modified parameters based on whether the drive is set for normal duty or heavy duty parameters.
</commit_message>
<xml_diff>
--- a/V1000_Drive_Programmer/data/DRIVE_LIST.xlsx
+++ b/V1000_Drive_Programmer/data/DRIVE_LIST.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="0" windowWidth="23025" windowHeight="7740"/>
+    <workbookView xWindow="4725" yWindow="0" windowWidth="23025" windowHeight="7740"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="30">
   <si>
     <t>Yaskawa</t>
   </si>
@@ -105,6 +105,15 @@
   </si>
   <si>
     <t>VARIABLE FREQUENCY DRIVE, 460V, 14.8 A</t>
+  </si>
+  <si>
+    <t>PARAM_HD_MOD</t>
+  </si>
+  <si>
+    <t>V1000_LV_HD_MODS</t>
+  </si>
+  <si>
+    <t>V1000_HV_HD_MODS</t>
   </si>
 </sst>
 </file>
@@ -421,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -435,10 +444,11 @@
     <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" customWidth="1"/>
+    <col min="8" max="8" width="18.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -458,10 +468,13 @@
         <v>13</v>
       </c>
       <c r="G1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -481,10 +494,13 @@
         <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -504,10 +520,13 @@
         <v>16</v>
       </c>
       <c r="G3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -527,10 +546,13 @@
         <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+      <c r="H4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -550,10 +572,13 @@
         <v>16</v>
       </c>
       <c r="G5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+      <c r="H5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -573,10 +598,13 @@
         <v>15</v>
       </c>
       <c r="G6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+      <c r="H6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -596,10 +624,13 @@
         <v>16</v>
       </c>
       <c r="G7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+      <c r="H7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -619,10 +650,13 @@
         <v>15</v>
       </c>
       <c r="G8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+      <c r="H8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -642,6 +676,9 @@
         <v>16</v>
       </c>
       <c r="G9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
In process of creating a method to verify the parameter list. I need to create a list of all the parameters with the modified values in there to verify the information that is read from the VFD against. Still in progress...
</commit_message>
<xml_diff>
--- a/V1000_Drive_Programmer/data/DRIVE_LIST.xlsx
+++ b/V1000_Drive_Programmer/data/DRIVE_LIST.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4725" yWindow="0" windowWidth="23025" windowHeight="7740"/>
+    <workbookView xWindow="5670" yWindow="0" windowWidth="23025" windowHeight="7740"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -107,13 +107,13 @@
     <t>VARIABLE FREQUENCY DRIVE, 460V, 14.8 A</t>
   </si>
   <si>
-    <t>PARAM_HD_MOD</t>
-  </si>
-  <si>
     <t>V1000_LV_HD_MODS</t>
   </si>
   <si>
     <t>V1000_HV_HD_MODS</t>
+  </si>
+  <si>
+    <t>PARAM_HD_MODS</t>
   </si>
 </sst>
 </file>
@@ -433,7 +433,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -444,7 +444,7 @@
     <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" customWidth="1"/>
+    <col min="7" max="7" width="19.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -468,7 +468,7 @@
         <v>13</v>
       </c>
       <c r="G1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H1" t="s">
         <v>14</v>
@@ -494,7 +494,7 @@
         <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H2" t="s">
         <v>17</v>
@@ -520,7 +520,7 @@
         <v>16</v>
       </c>
       <c r="G3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H3" t="s">
         <v>17</v>
@@ -546,7 +546,7 @@
         <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H4" t="s">
         <v>17</v>
@@ -572,7 +572,7 @@
         <v>16</v>
       </c>
       <c r="G5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H5" t="s">
         <v>17</v>
@@ -598,7 +598,7 @@
         <v>15</v>
       </c>
       <c r="G6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H6" t="s">
         <v>17</v>
@@ -624,7 +624,7 @@
         <v>16</v>
       </c>
       <c r="G7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H7" t="s">
         <v>17</v>
@@ -650,7 +650,7 @@
         <v>15</v>
       </c>
       <c r="G8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H8" t="s">
         <v>17</v>
@@ -676,7 +676,7 @@
         <v>16</v>
       </c>
       <c r="G9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H9" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Many changes that amount to being close to having a fully working programmer.
Still have problems with changing the drive selection not updating the Full Parameter List datagridview.

Added comboboxes and entry options for machine selection, supply voltage, supply frequency, and motor number. I plan on implementing this to work for machine selections.
</commit_message>
<xml_diff>
--- a/V1000_Drive_Programmer/data/DRIVE_LIST.xlsx
+++ b/V1000_Drive_Programmer/data/DRIVE_LIST.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5670" yWindow="0" windowWidth="23025" windowHeight="7740"/>
+    <workbookView xWindow="6615" yWindow="0" windowWidth="23025" windowHeight="7740"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,18 +65,9 @@
     <t>MFR_PARTNUM</t>
   </si>
   <si>
-    <t>PARAM_LIST</t>
-  </si>
-  <si>
     <t>PARAM_GRP_DESC</t>
   </si>
   <si>
-    <t>V1000_LIST_LV</t>
-  </si>
-  <si>
-    <t>V1000_LIST_HV</t>
-  </si>
-  <si>
     <t>V1000_GRP_DESC</t>
   </si>
   <si>
@@ -107,13 +98,22 @@
     <t>VARIABLE FREQUENCY DRIVE, 460V, 14.8 A</t>
   </si>
   <si>
-    <t>V1000_LV_HD_MODS</t>
-  </si>
-  <si>
-    <t>V1000_HV_HD_MODS</t>
-  </si>
-  <si>
-    <t>PARAM_HD_MODS</t>
+    <t>PARAM_ND_LIST</t>
+  </si>
+  <si>
+    <t>PARAM_HD_LIST</t>
+  </si>
+  <si>
+    <t>V1000_HV_ND</t>
+  </si>
+  <si>
+    <t>V1000_LV_ND</t>
+  </si>
+  <si>
+    <t>V1000_HV_HD</t>
+  </si>
+  <si>
+    <t>V1000_LV_HD</t>
   </si>
 </sst>
 </file>
@@ -433,7 +433,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -443,7 +443,7 @@
     <col min="3" max="3" width="38.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.44140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -456,7 +456,7 @@
         <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
         <v>11</v>
@@ -465,13 +465,13 @@
         <v>12</v>
       </c>
       <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
         <v>13</v>
-      </c>
-      <c r="G1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -482,7 +482,7 @@
         <v>21520</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -491,13 +491,13 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="G2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -508,7 +508,7 @@
         <v>21521</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -517,13 +517,13 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="G3" t="s">
         <v>28</v>
       </c>
       <c r="H3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -534,7 +534,7 @@
         <v>21522</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -543,13 +543,13 @@
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="G4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -560,7 +560,7 @@
         <v>21523</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -569,13 +569,13 @@
         <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="G5" t="s">
         <v>28</v>
       </c>
       <c r="H5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -586,7 +586,7 @@
         <v>21524</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -595,13 +595,13 @@
         <v>5</v>
       </c>
       <c r="F6" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="G6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -612,7 +612,7 @@
         <v>21525</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -621,13 +621,13 @@
         <v>6</v>
       </c>
       <c r="F7" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="G7" t="s">
         <v>28</v>
       </c>
       <c r="H7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -638,7 +638,7 @@
         <v>21540</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
         <v>0</v>
@@ -647,13 +647,13 @@
         <v>7</v>
       </c>
       <c r="F8" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="G8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -664,7 +664,7 @@
         <v>21541</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D9" t="s">
         <v>0</v>
@@ -673,13 +673,13 @@
         <v>8</v>
       </c>
       <c r="F9" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="G9" t="s">
         <v>28</v>
       </c>
       <c r="H9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Added code to warn user if they are trying to modify the VFD without setting up motor parameters. - Fixed the addition of motor parameters where setting the value in the datagridview for Scheduled Changes didn't show the correct setting.
</commit_message>
<xml_diff>
--- a/V1000_Drive_Programmer/data/DRIVE_LIST.xlsx
+++ b/V1000_Drive_Programmer/data/DRIVE_LIST.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6615" yWindow="0" windowWidth="23025" windowHeight="7740"/>
+    <workbookView xWindow="7560" yWindow="0" windowWidth="23025" windowHeight="7740"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="46">
   <si>
     <t>Yaskawa</t>
   </si>
@@ -104,16 +104,64 @@
     <t>PARAM_HD_LIST</t>
   </si>
   <si>
-    <t>V1000_HV_ND</t>
-  </si>
-  <si>
-    <t>V1000_LV_ND</t>
-  </si>
-  <si>
-    <t>V1000_HV_HD</t>
-  </si>
-  <si>
-    <t>V1000_LV_HD</t>
+    <t>VARIABLE FREQUENCY DRIVE, 230V, 3A</t>
+  </si>
+  <si>
+    <t>CIMR-VU2A0004BMA-092</t>
+  </si>
+  <si>
+    <t>21520_ND</t>
+  </si>
+  <si>
+    <t>21520_HD</t>
+  </si>
+  <si>
+    <t>21521_ND</t>
+  </si>
+  <si>
+    <t>21521_HD</t>
+  </si>
+  <si>
+    <t>21522_ND</t>
+  </si>
+  <si>
+    <t>21522_HD</t>
+  </si>
+  <si>
+    <t>21523_ND</t>
+  </si>
+  <si>
+    <t>21523_HD</t>
+  </si>
+  <si>
+    <t>21524_ND</t>
+  </si>
+  <si>
+    <t>21524_HD</t>
+  </si>
+  <si>
+    <t>21525_ND</t>
+  </si>
+  <si>
+    <t>21525_HD</t>
+  </si>
+  <si>
+    <t>21540_ND</t>
+  </si>
+  <si>
+    <t>21540_HD</t>
+  </si>
+  <si>
+    <t>21541_ND</t>
+  </si>
+  <si>
+    <t>21541_HD</t>
+  </si>
+  <si>
+    <t>21573_ND</t>
+  </si>
+  <si>
+    <t>21573_HD</t>
   </si>
 </sst>
 </file>
@@ -430,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -491,7 +539,7 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G2" t="s">
         <v>29</v>
@@ -517,10 +565,10 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="G3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="H3" t="s">
         <v>14</v>
@@ -543,10 +591,10 @@
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="G4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H4" t="s">
         <v>14</v>
@@ -569,10 +617,10 @@
         <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="G5" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="H5" t="s">
         <v>14</v>
@@ -595,10 +643,10 @@
         <v>5</v>
       </c>
       <c r="F6" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="G6" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="H6" t="s">
         <v>14</v>
@@ -621,10 +669,10 @@
         <v>6</v>
       </c>
       <c r="F7" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="G7" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="H7" t="s">
         <v>14</v>
@@ -647,10 +695,10 @@
         <v>7</v>
       </c>
       <c r="F8" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="G8" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="H8" t="s">
         <v>14</v>
@@ -673,12 +721,38 @@
         <v>8</v>
       </c>
       <c r="F9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>21573</v>
+      </c>
+      <c r="C10" t="s">
         <v>26</v>
       </c>
-      <c r="G9" t="s">
-        <v>28</v>
-      </c>
-      <c r="H9" t="s">
+      <c r="D10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>